<commit_message>
factor(one_file_one_tab): add delete methods
</commit_message>
<xml_diff>
--- a/fichiers_xls/listing_par_etape - Copie.xlsx
+++ b/fichiers_xls/listing_par_etape - Copie.xlsx
@@ -69,11 +69,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">

</xml_diff>